<commit_message>
feat: :sparkles: Rules checks and JSON simplification
</commit_message>
<xml_diff>
--- a/tests/material/database.xlsx
+++ b/tests/material/database.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="dates" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="object" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="listed" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="listed_simple" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="64">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -703,142 +704,262 @@
   </sheetPr>
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="0" t="s">
+      <c r="A9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="1" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="0" t="s">
+      <c r="A10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="1" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="0" t="s">
+      <c r="A11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="1" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="0" t="s">
+      <c r="A12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="1" t="s">
         <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="1" t="n">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: :bug: Complex rules and controls fixed
</commit_message>
<xml_diff>
--- a/tests/material/database.xlsx
+++ b/tests/material/database.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="66">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -137,7 +137,13 @@
     <t xml:space="preserve">&lt;20</t>
   </si>
   <si>
+    <t xml:space="preserve">algo</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">otro</t>
   </si>
   <si>
     <t xml:space="preserve">atb2</t>
@@ -573,10 +579,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -600,6 +606,9 @@
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="F1" s="0" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -617,6 +626,9 @@
       <c r="E2" s="1" t="n">
         <v>1.2</v>
       </c>
+      <c r="F2" s="0" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
@@ -629,10 +641,13 @@
         <v>35</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E3" s="1" t="n">
         <v>2.4</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -640,16 +655,19 @@
         <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>4.1</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -657,33 +675,39 @@
         <v>23</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E5" s="1" t="n">
         <v>4.2</v>
       </c>
+      <c r="F5" s="0" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>35</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E6" s="1" t="n">
         <v>7.2</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -726,10 +750,10 @@
         <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -737,10 +761,10 @@
         <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -748,10 +772,10 @@
         <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -759,10 +783,10 @@
         <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -770,10 +794,10 @@
         <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -781,10 +805,10 @@
         <v>19</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -792,10 +816,10 @@
         <v>23</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -803,10 +827,10 @@
         <v>25</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -814,10 +838,10 @@
         <v>25</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -825,10 +849,10 @@
         <v>25</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -836,10 +860,10 @@
         <v>25</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -860,7 +884,7 @@
   </sheetPr>
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>

</xml_diff>